<commit_message>
fix log in/out mechanism
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440B869F-6AF1-3946-AB1A-5107E461444E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F868B09-ABDF-41E5-914C-ED51B1BB4EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
+    <sheet name="Scouting Admin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Feature</t>
   </si>
@@ -83,10 +84,10 @@
     <t>Edit Question</t>
   </si>
   <si>
-    <t>View Question Table with row click action</t>
-  </si>
-  <si>
     <t>Team Contact Form</t>
+  </si>
+  <si>
+    <t>View Response Table with row click action</t>
   </si>
 </sst>
 </file>
@@ -129,14 +130,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,16 +453,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316C606-7CAE-2E44-BE5B-D70A1C25ECB4}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:B15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,14 +473,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -488,7 +488,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -496,7 +496,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -504,7 +504,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -512,100 +512,167 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="3">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" s="1">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="B9" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="4">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="4">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B16" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="4">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2">
         <v>45314</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="A15:C15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05D928-9B9A-4488-A796-28AB47990C24}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45314</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
     <mergeCell ref="A2:C2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
too many, but highlight new screen size sys
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F868B09-ABDF-41E5-914C-ED51B1BB4EB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D74A6A-0182-41AF-8E6F-FEDD895801D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Feature</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Manage Users</t>
   </si>
   <si>
-    <t>User Table Main Display Edit Capabilities</t>
-  </si>
-  <si>
     <t>Manage Users Modal</t>
   </si>
   <si>
@@ -88,6 +85,27 @@
   </si>
   <si>
     <t>View Response Table with row click action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scout Field Schedule Table </t>
+  </si>
+  <si>
+    <t>Scout Field Schedule Modal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Save</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Edit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Copy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Delete</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Notify</t>
   </si>
 </sst>
 </file>
@@ -451,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316C606-7CAE-2E44-BE5B-D70A1C25ECB4}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C6"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -505,34 +523,33 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
-        <v>45314</v>
-      </c>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
+      <c r="B7" s="1">
+        <v>45314</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>45314</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
-        <v>45314</v>
-      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -542,11 +559,12 @@
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="2">
+        <v>45314</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -558,26 +576,26 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="2">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="2">
-        <v>45314</v>
-      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2">
+        <v>45314</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -589,27 +607,19 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>45314</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2">
         <v>45314</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
     <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -617,10 +627,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05D928-9B9A-4488-A796-28AB47990C24}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -660,15 +670,60 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
-        <v>45314</v>
+        <v>45315</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>45314</v>
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix button col width
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E989DAB9-4AF5-45FF-B940-0ECFD33BFE2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE76E6F0-2BDA-5743-9C03-B466773CFDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -514,12 +514,12 @@
       <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -530,14 +530,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -545,7 +545,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -553,7 +553,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -561,13 +561,13 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -575,7 +575,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -583,21 +583,21 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -605,7 +605,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -613,7 +613,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -621,14 +621,14 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -636,7 +636,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -644,7 +644,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -672,13 +672,13 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,14 +689,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -704,7 +704,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -712,7 +712,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -720,7 +720,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -728,7 +728,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -736,7 +736,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -744,7 +744,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -752,7 +752,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -760,19 +760,19 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -780,7 +780,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -788,7 +788,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -796,7 +796,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -804,7 +804,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -812,7 +812,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -820,17 +820,23 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -838,7 +844,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -846,7 +852,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -854,7 +860,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
phone type clean up
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE76E6F0-2BDA-5743-9C03-B466773CFDA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30CBC70-0CC5-6E40-B0AB-E1285E7ED56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
   <si>
     <t>Feature</t>
   </si>
@@ -145,6 +145,21 @@
   </si>
   <si>
     <t>Remove Team From Event</t>
+  </si>
+  <si>
+    <t>Field Questions</t>
+  </si>
+  <si>
+    <t>Save</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Pit Questions</t>
+  </si>
+  <si>
+    <t>Phone Types</t>
   </si>
 </sst>
 </file>
@@ -666,10 +681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05D928-9B9A-4488-A796-28AB47990C24}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A32" sqref="A32:B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -804,7 +819,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -812,7 +827,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -820,7 +835,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -828,7 +843,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -836,7 +851,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -844,7 +859,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -852,7 +867,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -860,7 +875,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -868,10 +883,82 @@
         <v>45317</v>
       </c>
     </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="1">
+        <v>45317</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
split out schedules in portal
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30CBC70-0CC5-6E40-B0AB-E1285E7ED56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606233DC-016D-FE4F-B205-15FDDE8A82A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Scouting Admin" sheetId="2" r:id="rId2"/>
+    <sheet name="Portal" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -683,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05D928-9B9A-4488-A796-28AB47990C24}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A32" sqref="A32:B33"/>
     </sheetView>
   </sheetViews>
@@ -963,4 +964,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00FE40B-736F-1F44-980E-E4212B605D3E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix multi select constant model change event
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CD7E2D-36BA-FB44-9A4E-4C1EAAED2AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BBA6F1E-840E-1547-8926-27D2F239D34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
     <sheet name="Scouting Admin" sheetId="2" r:id="rId2"/>
     <sheet name="Portal" sheetId="3" r:id="rId3"/>
+    <sheet name="Field Scouting" sheetId="4" r:id="rId4"/>
+    <sheet name="Scout Field Results" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Feature</t>
   </si>
@@ -185,6 +187,12 @@
   </si>
   <si>
     <t>Copy</t>
+  </si>
+  <si>
+    <t>Field Schedule</t>
+  </si>
+  <si>
+    <t>Auto Team Select By Match</t>
   </si>
 </sst>
 </file>
@@ -994,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D00FE40B-736F-1F44-980E-E4212B605D3E}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1078,4 +1086,95 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E68718-366B-E24C-AE47-0AA1795EF282}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CD69FE-93D4-064B-B1A0-4A54E5B1A923}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
move notes to sub nav
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80BF44DB-9610-5B46-8999-EEF3F7BC7758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FCAAFE-345E-EE49-BBD8-E57466675C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Feature</t>
   </si>
@@ -217,6 +217,12 @@
   </si>
   <si>
     <t>Row click for results</t>
+  </si>
+  <si>
+    <t>take note</t>
+  </si>
+  <si>
+    <t>view notes</t>
   </si>
 </sst>
 </file>
@@ -1312,10 +1318,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FF00A8-7F8C-D240-B060-523E745943A9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1350,6 +1356,22 @@
         <v>45323</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45323</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix null on save
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brandon/git/PARTs_Website/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FCAAFE-345E-EE49-BBD8-E57466675C9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00470A59-E946-4C1A-A9FC-4401C012F790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="7" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -290,9 +290,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -330,7 +330,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -436,7 +436,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -578,7 +578,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -586,18 +586,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7316C606-7CAE-2E44-BE5B-D70A1C25ECB4}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,14 +608,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -623,7 +623,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -631,7 +631,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -639,13 +639,13 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -653,7 +653,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -661,21 +661,21 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -683,7 +683,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -691,7 +691,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -699,14 +699,14 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -714,7 +714,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -722,7 +722,7 @@
         <v>45314</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -730,8 +730,32 @@
         <v>45314</v>
       </c>
     </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="1">
+        <v>45317</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A9:C9"/>
@@ -744,19 +768,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05D928-9B9A-4488-A796-28AB47990C24}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="A31" sqref="A31:C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -767,14 +791,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -782,7 +806,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -790,7 +814,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -798,7 +822,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -806,7 +830,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -814,7 +838,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -822,7 +846,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -830,7 +854,7 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -838,19 +862,19 @@
         <v>45315</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -858,7 +882,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -866,7 +890,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -874,7 +898,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -882,7 +906,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -890,7 +914,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -898,7 +922,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -906,7 +930,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -914,7 +938,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -922,7 +946,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -930,7 +954,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -938,7 +962,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -946,14 +970,14 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -961,7 +985,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
@@ -969,14 +993,14 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -984,7 +1008,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -992,36 +1016,12 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="1">
-        <v>45317</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="1">
-        <v>45317</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1036,12 +1036,12 @@
       <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>46</v>
       </c>
@@ -1100,12 +1100,12 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -1126,12 +1126,12 @@
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -1166,16 +1166,16 @@
         <v>45317</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
   </sheetData>
@@ -1191,9 +1191,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1217,13 +1217,13 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1234,7 +1234,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1261,7 +1261,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -1282,9 +1282,9 @@
       <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>45322</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1320,16 +1320,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FF00A8-7F8C-D240-B060-523E745943A9}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
@@ -1356,7 +1356,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -1364,7 +1364,7 @@
         <v>45323</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
working on check in
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723CA577-D202-4DB7-A189-DEAB27EB2BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ABCB25-4B9C-4821-8574-A9E326365B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="1" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="80">
   <si>
     <t>Feature</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Delete Event</t>
   </si>
   <si>
-    <t>Add Event</t>
-  </si>
-  <si>
     <t>Add Team</t>
   </si>
   <si>
@@ -282,6 +279,15 @@
   </si>
   <si>
     <t>Field Scouting Schedule</t>
+  </si>
+  <si>
+    <t>Add TBA Code Event</t>
+  </si>
+  <si>
+    <t>Add Event manual input</t>
+  </si>
+  <si>
+    <t>Need to fix</t>
   </si>
 </sst>
 </file>
@@ -684,7 +690,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="1">
         <v>45412</v>
@@ -692,13 +698,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1">
         <v>45412</v>
@@ -706,7 +712,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1">
         <v>45412</v>
@@ -714,7 +720,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B9" s="1">
         <v>45412</v>
@@ -722,7 +728,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B10" s="1">
         <v>45412</v>
@@ -730,7 +736,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B11" s="1">
         <v>45412</v>
@@ -738,7 +744,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B12" s="1">
         <v>45412</v>
@@ -746,7 +752,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B13" s="1">
         <v>45412</v>
@@ -754,7 +760,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="1">
         <v>45412</v>
@@ -824,14 +830,14 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="1">
         <v>45412</v>
@@ -839,7 +845,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B25" s="1">
         <v>45412</v>
@@ -939,10 +945,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A05D928-9B9A-4488-A796-28AB47990C24}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -979,7 +985,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1">
         <v>45412</v>
@@ -997,7 +1003,7 @@
         <v>23</v>
       </c>
       <c r="B6" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1005,7 +1011,7 @@
         <v>24</v>
       </c>
       <c r="B7" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1013,7 +1019,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1021,7 +1027,7 @@
         <v>26</v>
       </c>
       <c r="B9" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1029,7 +1035,7 @@
         <v>27</v>
       </c>
       <c r="B10" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1037,7 +1043,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1045,7 +1051,7 @@
         <v>29</v>
       </c>
       <c r="B12" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1053,59 +1059,62 @@
         <v>30</v>
       </c>
       <c r="B13" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="B14" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>78</v>
       </c>
       <c r="B15" s="1">
-        <v>45317</v>
+        <v>45412</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B16" s="1">
-        <v>45317</v>
+        <v>31</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="1">
-        <v>45317</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>15</v>
-      </c>
-      <c r="B19" s="1">
-        <v>45315</v>
-      </c>
+      <c r="A19" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B20" s="1">
         <v>45315</v>
@@ -1113,7 +1122,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1">
         <v>45315</v>
@@ -1121,7 +1130,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
         <v>45315</v>
@@ -1129,7 +1138,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="1">
         <v>45315</v>
@@ -1137,7 +1146,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B24" s="1">
         <v>45315</v>
@@ -1145,110 +1154,118 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28" s="1">
-        <v>45317</v>
-      </c>
+      <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" s="1">
         <v>45317</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="1">
+        <v>45317</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34" s="1">
-        <v>45317</v>
-      </c>
+      <c r="A34" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="1">
         <v>45317</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1">
+        <v>45317</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A33:C33"/>
     <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A30:C30"/>
-    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1281,7 +1298,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="1">
         <v>45317</v>
@@ -1289,7 +1306,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1">
         <v>45317</v>
@@ -1297,7 +1314,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1">
         <v>45317</v>
@@ -1305,7 +1322,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="1">
         <v>45317</v>
@@ -1313,7 +1330,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="1">
         <v>45317</v>
@@ -1321,7 +1338,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1">
         <v>45317</v>
@@ -1329,12 +1346,12 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1">
         <v>45317</v>
@@ -1371,7 +1388,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="1">
         <v>45317</v>
@@ -1379,7 +1396,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1">
         <v>45317</v>
@@ -1387,7 +1404,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1">
         <v>45317</v>
@@ -1463,7 +1480,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="1">
         <v>45322</v>
@@ -1471,7 +1488,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1">
         <v>45322</v>
@@ -1479,18 +1496,18 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="1">
         <v>45322</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="1">
         <v>45322</v>
@@ -1524,7 +1541,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1">
         <v>45322</v>
@@ -1532,7 +1549,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="1">
         <v>45322</v>
@@ -1569,7 +1586,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>45323</v>
@@ -1577,7 +1594,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="1">
         <v>45323</v>
@@ -1585,7 +1602,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="1">
         <v>45323</v>
@@ -1593,7 +1610,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B5" s="1">
         <v>45323</v>

</xml_diff>

<commit_message>
fix color to team
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4504A11-AE9A-4EB1-884F-69231AA0F60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BC96EA-5542-401F-95E6-836000BF8C0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="10" activeTab="12" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="10" activeTab="11" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,12 @@
     <sheet name="Competition Page" sheetId="17" r:id="rId9"/>
     <sheet name="Contact" sheetId="9" r:id="rId10"/>
     <sheet name="Application Form" sheetId="10" r:id="rId11"/>
-    <sheet name="Notifications" sheetId="11" r:id="rId12"/>
-    <sheet name="Messages" sheetId="12" r:id="rId13"/>
-    <sheet name="User Profile" sheetId="13" r:id="rId14"/>
-    <sheet name="Question Conditions" sheetId="14" r:id="rId15"/>
-    <sheet name="Question Aggregates" sheetId="15" r:id="rId16"/>
-    <sheet name="Alerts" sheetId="16" r:id="rId17"/>
+    <sheet name="Alerts" sheetId="16" r:id="rId12"/>
+    <sheet name="Notifications in app" sheetId="11" r:id="rId13"/>
+    <sheet name="Messages in app" sheetId="12" r:id="rId14"/>
+    <sheet name="User Profile" sheetId="13" r:id="rId15"/>
+    <sheet name="Question Conditions" sheetId="14" r:id="rId16"/>
+    <sheet name="Question Aggregates" sheetId="15" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="107">
   <si>
     <t>Feature</t>
   </si>
@@ -346,6 +346,33 @@
   </si>
   <si>
     <t>Match schedule</t>
+  </si>
+  <si>
+    <t>5 min field schedule alert</t>
+  </si>
+  <si>
+    <t>15 min field schedule alert</t>
+  </si>
+  <si>
+    <t>time of field schedule alert</t>
+  </si>
+  <si>
+    <t>late scout alert, every 5 mins past time</t>
+  </si>
+  <si>
+    <t>commented out atm</t>
+  </si>
+  <si>
+    <t>Stage Alerts</t>
+  </si>
+  <si>
+    <t>schedule alerts for pit</t>
+  </si>
+  <si>
+    <t>Missing field response alert</t>
+  </si>
+  <si>
+    <t>Send Alerts</t>
   </si>
 </sst>
 </file>
@@ -388,10 +415,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,11 +757,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -761,10 +788,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="3"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -831,11 +858,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -862,11 +889,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -893,11 +920,11 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="A23" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -916,10 +943,10 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B26" s="3"/>
+      <c r="B26" s="4"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -938,11 +965,11 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="A29" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1001,7 +1028,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1034,22 +1061,129 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E562925-24EB-4C58-959C-0A692819837E}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE01F3-4A2E-4576-BCEF-BDC19AE162FF}">
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="33.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99488F6-2534-437C-A3A4-C67E3CB7A6D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E562925-24EB-4C58-959C-0A692819837E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1058,6 +1192,18 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99488F6-2534-437C-A3A4-C67E3CB7A6D9}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F4966F-DC12-4D07-8FD8-FD681CF3B0FC}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1069,7 +1215,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC432B19-E382-4340-8804-1D8D0E79A8F1}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1083,25 +1229,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876D4F33-167B-462C-8457-D155EEA71F92}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03DE01F3-4A2E-4576-BCEF-BDC19AE162FF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -1135,11 +1267,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1158,11 +1290,11 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1272,11 +1404,11 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1335,11 +1467,11 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1398,14 +1530,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B36" s="1">
@@ -1414,7 +1546,7 @@
       <c r="C36" s="2"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>75</v>
       </c>
       <c r="B37" s="1">
@@ -1423,7 +1555,7 @@
       <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="3" t="s">
         <v>77</v>
       </c>
       <c r="B38" s="1">
@@ -1432,7 +1564,7 @@
       <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+      <c r="A39" s="3" t="s">
         <v>76</v>
       </c>
       <c r="B39" s="1">
@@ -1441,7 +1573,7 @@
       <c r="C39" s="2"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="3" t="s">
         <v>78</v>
       </c>
       <c r="B40" s="1">
@@ -1450,11 +1582,11 @@
       <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -1473,11 +1605,11 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
+      <c r="A44" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
@@ -1496,11 +1628,11 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+      <c r="A47" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
@@ -1508,14 +1640,14 @@
       <c r="C48" s="2"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="4"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B50" s="1">
@@ -1524,11 +1656,11 @@
       <c r="C50" s="2"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="3"/>
+      <c r="B51" s="4"/>
+      <c r="C51" s="4"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
@@ -1547,11 +1679,11 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -1570,14 +1702,14 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="A57" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="3"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="4"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>79</v>
       </c>
       <c r="B58" s="1">

</xml_diff>

<commit_message>
add time delay to upload resutls
</commit_message>
<xml_diff>
--- a/Features.xlsx
+++ b/Features.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brandon\git\PARTs_Website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D6D88C-C63B-4487-9B95-4144120B44FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F735FE32-81D0-4BCE-A02C-7850F105DA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" firstSheet="10" activeTab="13" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" activeTab="6" xr2:uid="{C9A31F1F-8F92-6644-897E-F1AA069F5DE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="129">
   <si>
     <t>Feature</t>
   </si>
@@ -403,6 +403,42 @@
   </si>
   <si>
     <t>view all mesages button</t>
+  </si>
+  <si>
+    <t>Change profile image</t>
+  </si>
+  <si>
+    <t>not implemented</t>
+  </si>
+  <si>
+    <t>view notifications</t>
+  </si>
+  <si>
+    <t>dismiss notificaitons</t>
+  </si>
+  <si>
+    <t>view messages</t>
+  </si>
+  <si>
+    <t>dismiss messages</t>
+  </si>
+  <si>
+    <t>change information in general</t>
+  </si>
+  <si>
+    <t>change password</t>
+  </si>
+  <si>
+    <t>question can have multiple conditions</t>
+  </si>
+  <si>
+    <t>if a question is a contition it can only belong to one question</t>
+  </si>
+  <si>
+    <t>Offline</t>
+  </si>
+  <si>
+    <t>Results upload when online</t>
   </si>
 </sst>
 </file>
@@ -1291,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99488F6-2534-437C-A3A4-C67E3CB7A6D9}">
   <dimension ref="A31:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1351,38 +1387,159 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6F4966F-DC12-4D07-8FD8-FD681CF3B0FC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B4" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC432B19-E382-4340-8804-1D8D0E79A8F1}">
-  <dimension ref="A1"/>
+  <dimension ref="A16:C18"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="51.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{876D4F33-167B-462C-8457-D155EEA71F92}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1887,7 +2044,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1931,25 +2088,51 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="A5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45412</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45412</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77E68718-366B-E24C-AE47-0AA1795EF282}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2001,28 +2184,64 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
+      <c r="A6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45412</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="1"/>
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45412</v>
+      </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" s="1"/>
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>128</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15CD69FE-93D4-064B-B1A0-4A54E5B1A923}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A11" sqref="A11:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2113,17 +2332,83 @@
         <v>45412</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>90</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="1">
+        <v>45412</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A11:C11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83F51E54-1133-3E40-B992-FB47DDB905A7}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2178,17 +2463,51 @@
         <v>45412</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45412</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>128</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A6:C6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D750F959-D19E-A044-B3B1-8D2A997D08EB}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2231,7 +2550,33 @@
         <v>45412</v>
       </c>
     </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1">
+        <v>45412</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1">
+        <v>45412</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A5:C5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>